<commit_message>
adjusting etl pipeline files and adding new files to help with the execution of the pipeline
</commit_message>
<xml_diff>
--- a/data/input/employee_absence_data_0.xlsx
+++ b/data/input/employee_absence_data_0.xlsx
@@ -464,292 +464,292 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>89857</v>
+        <v>14405</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Maria Isis Alves</t>
+          <t>Alícia Pires</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vendas</t>
+          <t>Engenharia</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Doenca</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>45085</v>
+        <v>45082</v>
       </c>
       <c r="G2" t="n">
-        <v>6873.5</v>
+        <v>2709.93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>42285</v>
+        <v>82326</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Julia Cunha</t>
+          <t>Breno Rocha</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>P&amp;D</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Viagem de negocios</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>45102</v>
+        <v>45096</v>
       </c>
       <c r="G3" t="n">
-        <v>7115.94</v>
+        <v>3458.02</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>16062</v>
+        <v>34256</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dra. Maria Isis Azevedo</t>
+          <t>Luiza Pacheco</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Vendas</t>
+          <t>Financeiro</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Consulta medica</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>45098</v>
+        <v>45089</v>
       </c>
       <c r="G4" t="n">
-        <v>3794.01</v>
+        <v>3361.77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>12745</v>
+        <v>47345</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ian da Luz</t>
+          <t>Maria Liz Moura</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Vendas</t>
+          <t>Atendimento ao Cliente</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Consulta medica</t>
+          <t>Viagem de negocios</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>45081</v>
+        <v>45088</v>
       </c>
       <c r="G5" t="n">
-        <v>10965.68</v>
+        <v>8832.309999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>93058</v>
+        <v>6113</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cecilia Ferreira</t>
+          <t>Dr. Cauã Gomes</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Operacoes</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Viagem de negocios</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E6" t="n">
         <v>4</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>45091</v>
+        <v>45089</v>
       </c>
       <c r="G6" t="n">
-        <v>4278.06</v>
+        <v>9343.120000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>94053</v>
+        <v>84876</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Esther Pacheco</t>
+          <t>Dra. Cecília da Rosa</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Financeiro</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Doenca</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>45091</v>
+        <v>45092</v>
       </c>
       <c r="G7" t="n">
-        <v>8595.200000000001</v>
+        <v>4041.16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>77940</v>
+        <v>27234</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sra. Marcela Costela</t>
+          <t>Melina Dias</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Operacoes</t>
+          <t>P&amp;D</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Consulta medica</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E8" t="n">
         <v>3</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>45100</v>
+        <v>45094</v>
       </c>
       <c r="G8" t="n">
-        <v>2824.36</v>
+        <v>6078.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>88428</v>
+        <v>2131</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sra. Emanuella da Cruz</t>
+          <t>Maria Isis Cassiano</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Juridico</t>
+          <t>P&amp;D</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Consulta medica</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>45078</v>
+        <v>45104</v>
       </c>
       <c r="G9" t="n">
-        <v>3079.39</v>
+        <v>2349.19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>35176</v>
+        <v>31710</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Brenda Araújo</t>
+          <t>Lavínia Aparecida</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Atendimento ao Cliente</t>
+          <t>Vendas</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Consulta medica</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>45079</v>
+        <v>45091</v>
       </c>
       <c r="G10" t="n">
-        <v>6974.81</v>
+        <v>7535.09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4515</v>
+        <v>4192</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Yago Silva</t>
+          <t>Marcela Costela</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Operacoes</t>
+          <t>Atendimento ao Cliente</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Viagem de negocios</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>45078</v>
+        <v>45106</v>
       </c>
       <c r="G11" t="n">
-        <v>5190.54</v>
+        <v>9869.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding taskipy tasks and adjusting files
</commit_message>
<xml_diff>
--- a/data/input/employee_absence_data_0.xlsx
+++ b/data/input/employee_absence_data_0.xlsx
@@ -464,16 +464,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>14405</v>
+        <v>65071</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alícia Pires</t>
+          <t>Luiz Gustavo Barros</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Engenharia</t>
+          <t>Recursos Humanos</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -482,254 +482,254 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>45082</v>
+        <v>45096</v>
       </c>
       <c r="G2" t="n">
-        <v>2709.93</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>82326</v>
+        <v>64824</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Breno Rocha</t>
+          <t>Ana Júlia Andrade</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>P&amp;D</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>45096</v>
+        <v>45104</v>
       </c>
       <c r="G3" t="n">
-        <v>3458.02</v>
+        <v>2259.55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>34256</v>
+        <v>52874</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Luiza Pacheco</t>
+          <t>Manuela Lima</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Financeiro</t>
+          <t>Operacoes</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Consulta medica</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>45089</v>
+        <v>45091</v>
       </c>
       <c r="G4" t="n">
-        <v>3361.77</v>
+        <v>3651.48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>47345</v>
+        <v>43213</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Maria Liz Moura</t>
+          <t>Maria Júlia Sá</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Atendimento ao Cliente</t>
+          <t>Juridico</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Viagem de negocios</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>45088</v>
+        <v>45098</v>
       </c>
       <c r="G5" t="n">
-        <v>8832.309999999999</v>
+        <v>5707.72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6113</v>
+        <v>49712</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dr. Cauã Gomes</t>
+          <t>Maria Liz Ferreira</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Operacoes</t>
+          <t>P&amp;D</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Consulta medica</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>45089</v>
+        <v>45087</v>
       </c>
       <c r="G6" t="n">
-        <v>9343.120000000001</v>
+        <v>6110.01</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>84876</v>
+        <v>74651</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dra. Cecília da Rosa</t>
+          <t>Augusto Casa Grande</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Financeiro</t>
+          <t>Engenharia</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Doenca</t>
+          <t>Consulta medica</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>45092</v>
+        <v>45079</v>
       </c>
       <c r="G7" t="n">
-        <v>4041.16</v>
+        <v>8154.67</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>27234</v>
+        <v>30076</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Melina Dias</t>
+          <t>Sarah Gonçalves</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>P&amp;D</t>
+          <t>Engenharia</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Consulta medica</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>45094</v>
+        <v>45101</v>
       </c>
       <c r="G8" t="n">
-        <v>6078.2</v>
+        <v>6421.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2131</v>
+        <v>84085</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Maria Isis Cassiano</t>
+          <t>Ester Siqueira</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>P&amp;D</t>
+          <t>Juridico</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Viagem de negocios</t>
         </is>
       </c>
       <c r="E9" t="n">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>45104</v>
+        <v>45088</v>
       </c>
       <c r="G9" t="n">
-        <v>2349.19</v>
+        <v>5896.46</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>31710</v>
+        <v>49142</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lavínia Aparecida</t>
+          <t>Srta. Ágatha da Luz</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Vendas</t>
+          <t>Engenharia</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Viagem de negocios</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>45091</v>
+        <v>45093</v>
       </c>
       <c r="G10" t="n">
-        <v>7535.09</v>
+        <v>8480.92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4192</v>
+        <v>79804</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Marcela Costela</t>
+          <t>Sr. Diego Sampaio</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -739,17 +739,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Doenca</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>45106</v>
+        <v>45078</v>
       </c>
       <c r="G11" t="n">
-        <v>9869.6</v>
+        <v>8412.790000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>